<commit_message>
Update 4h18 PM 01-10-2025
</commit_message>
<xml_diff>
--- a/DATA/Book1.xlsx
+++ b/DATA/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OTHER\DU_AN_CA_NHAN_WEB_BAN_DT\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7CEB04-C990-48B9-83D3-59C0FFC530D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8118B03B-03A9-4526-B61F-CD18CC6851AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B9135E77-B1C7-47E3-9CAA-85984D8E6277}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="605">
   <si>
     <t>Product</t>
   </si>
@@ -1831,6 +1831,24 @@
   </si>
   <si>
     <t>detail_total_price</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>blog_id</t>
+  </si>
+  <si>
+    <t>blog_name</t>
+  </si>
+  <si>
+    <t>blog_author</t>
+  </si>
+  <si>
+    <t>blog_link</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -2626,10 +2644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB60E5F-678A-47BD-9DEC-6DA2588FD9D6}">
-  <dimension ref="B4:H85"/>
+  <dimension ref="B4:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3431,6 +3449,53 @@
       </c>
       <c r="E85" s="8" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B88" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C89" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C90" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C91" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>